<commit_message>
Defined client class and executed unit test
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_bank_account.xlsx
+++ b/tests/A01_pixell_test_plan_bank_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\2. Assignments\updated_again_0416\assignment_01\starter (given)\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c3d6174ceab06f3/Desktop/rrc_polytech/courses_term2/intermediate_software_development/project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DA4A4F-2E79-4753-B9BE-A428E4C99413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{56DA4A4F-2E79-4753-B9BE-A428E4C99413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{234B5A4E-3D94-4EDB-BD69-793E08589702}"/>
   <bookViews>
-    <workbookView xWindow="31140" yWindow="2340" windowWidth="25185" windowHeight="13845" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -282,6 +282,87 @@
   </si>
   <si>
     <t>returns client number attribute</t>
+  </si>
+  <si>
+    <t>Jashanpreet Kaur Jattana</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>account_number=12345, client_number=67890, balance=500.0</t>
+  </si>
+  <si>
+    <t>account_number=12345, client_number=67890, balance=500.00</t>
+  </si>
+  <si>
+    <t>BankAccount object with account_number=12345</t>
+  </si>
+  <si>
+    <t>BankAccount object with client_number=67890</t>
+  </si>
+  <si>
+    <t>BankAccount object with balance=500.0</t>
+  </si>
+  <si>
+    <t>account_number=12345, client_number=67890, balance="abc"</t>
+  </si>
+  <si>
+    <t>account_number="abc", client_number=67890, balance=500.0</t>
+  </si>
+  <si>
+    <t>account_number=12345, client_number="abc", balance=500.0</t>
+  </si>
+  <si>
+    <t>amount=100.0</t>
+  </si>
+  <si>
+    <t>amount="abc"</t>
+  </si>
+  <si>
+    <t>amount=-50.0</t>
+  </si>
+  <si>
+    <t>amount=200.0</t>
+  </si>
+  <si>
+    <t>amount=600.0</t>
+  </si>
+  <si>
+    <t>Balance should be set to 0.0</t>
+  </si>
+  <si>
+    <t>ValueError because account_number must be an integer</t>
+  </si>
+  <si>
+    <t>ValueError because client_number must be an integer</t>
+  </si>
+  <si>
+    <t>Updated balance should be 600.0</t>
+  </si>
+  <si>
+    <t>Updated balance should be 450.0</t>
+  </si>
+  <si>
+    <t>Balance should remain 500.0</t>
+  </si>
+  <si>
+    <t>Updated balance should be 700.0</t>
+  </si>
+  <si>
+    <t>ValueError because deposit amount must be positive</t>
+  </si>
+  <si>
+    <t>Updated balance should be 300.0</t>
+  </si>
+  <si>
+    <t>ValueError because withdrawl amount must be positive</t>
+  </si>
+  <si>
+    <t>ValueError because withdrawl amount must not exceed the current balance</t>
+  </si>
+  <si>
+    <t>"Account Number: 12345 Balance: 500"</t>
   </si>
 </sst>
 </file>
@@ -619,6 +700,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -642,12 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1193,53 +1274,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1259,21 +1342,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1283,25 +1372,37 @@
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13">
         <v>3</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10">
         <v>4</v>
       </c>
@@ -1311,25 +1412,37 @@
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="12">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10">
         <v>6</v>
       </c>
@@ -1339,25 +1452,37 @@
       <c r="D12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="12">
+        <v>67890</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>7</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
         <v>8</v>
       </c>
@@ -1367,25 +1492,37 @@
       <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10">
         <v>9</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10">
         <v>10</v>
       </c>
@@ -1395,25 +1532,37 @@
       <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <v>11</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>12</v>
       </c>
@@ -1423,25 +1572,37 @@
       <c r="D18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="13">
         <v>13</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="10">
         <v>14</v>
       </c>
@@ -1451,25 +1612,37 @@
       <c r="D20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10">
         <v>15</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>16</v>
       </c>
@@ -1479,11 +1652,17 @@
       <c r="D22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1493,7 +1672,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>18</v>
       </c>
@@ -1503,7 +1682,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10">
         <v>19</v>
       </c>
@@ -1513,7 +1692,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="10">
         <v>20</v>
       </c>
@@ -1523,7 +1702,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>21</v>
       </c>
@@ -1533,7 +1712,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>22</v>
       </c>
@@ -1543,7 +1722,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="13">
         <v>23</v>
       </c>
@@ -1553,7 +1732,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="10">
         <v>24</v>
       </c>
@@ -1563,7 +1742,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="10">
         <v>25</v>
       </c>
@@ -1573,7 +1752,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>26</v>
       </c>
@@ -1583,7 +1762,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>27</v>
       </c>
@@ -1593,7 +1772,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="13">
         <v>28</v>
       </c>
@@ -1603,7 +1782,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="10">
         <v>29</v>
       </c>
@@ -1613,7 +1792,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="10">
         <v>30</v>
       </c>
@@ -1623,7 +1802,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="10">
         <v>31</v>
       </c>
@@ -1633,15 +1812,15 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>